<commit_message>
Update Technical Resource Tracking.xlsx
added mass and time for production on versions
</commit_message>
<xml_diff>
--- a/Systems Engineering/Phase B - Preliminary Design and Technology Completition/Technical Resource Tracking.xlsx
+++ b/Systems Engineering/Phase B - Preliminary Design and Technology Completition/Technical Resource Tracking.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brand\Documents\RC-Plane\Systems Engineering\Phase B - Preliminary Design and Technology Completition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272FF56D-4E6C-4BF0-AD7D-9141241C879F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F550E0C-B251-4860-B454-7BA3DAC818FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mass Budget" sheetId="1" r:id="rId1"/>
-    <sheet name="Cost" sheetId="2" r:id="rId2"/>
+    <sheet name="Wing Mass and Time" sheetId="3" r:id="rId2"/>
+    <sheet name="Body Mass and Time" sheetId="4" r:id="rId3"/>
+    <sheet name="Cost" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="99">
   <si>
     <t>Object</t>
   </si>
@@ -160,13 +162,187 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>Print Object</t>
+  </si>
+  <si>
+    <t>Version 1</t>
+  </si>
+  <si>
+    <t>Mass</t>
+  </si>
+  <si>
+    <t>Version 2</t>
+  </si>
+  <si>
+    <t>Mass w/ Support</t>
+  </si>
+  <si>
+    <t>Rib 2</t>
+  </si>
+  <si>
+    <t>Rib 4</t>
+  </si>
+  <si>
+    <t>Rib 5</t>
+  </si>
+  <si>
+    <t>Rib 3</t>
+  </si>
+  <si>
+    <t>Rib 6</t>
+  </si>
+  <si>
+    <t>Rib 7</t>
+  </si>
+  <si>
+    <t>Rib 8</t>
+  </si>
+  <si>
+    <t>Wing</t>
+  </si>
+  <si>
+    <t>11/1:35</t>
+  </si>
+  <si>
+    <t>5/0:46</t>
+  </si>
+  <si>
+    <t>5/0:41</t>
+  </si>
+  <si>
+    <t>12/1:42</t>
+  </si>
+  <si>
+    <t>11/1:38</t>
+  </si>
+  <si>
+    <t>33/5:07</t>
+  </si>
+  <si>
+    <t>35/6:09</t>
+  </si>
+  <si>
+    <t>Servo Mount</t>
+  </si>
+  <si>
+    <t>21/3:09</t>
+  </si>
+  <si>
+    <t>19/2:55</t>
+  </si>
+  <si>
+    <t>Front Inner Spar</t>
+  </si>
+  <si>
+    <t>6/0:49</t>
+  </si>
+  <si>
+    <t>Front Mid Spar</t>
+  </si>
+  <si>
+    <t>9/1:08</t>
+  </si>
+  <si>
+    <t>Front Outer Spar</t>
+  </si>
+  <si>
+    <t>6/0:47</t>
+  </si>
+  <si>
+    <t>Leading Edge Outer</t>
+  </si>
+  <si>
+    <t>5/0:45</t>
+  </si>
+  <si>
+    <t>Leading Edge Inner</t>
+  </si>
+  <si>
+    <t>Leading Edge Mid (5x)</t>
+  </si>
+  <si>
+    <t>24/4:01</t>
+  </si>
+  <si>
+    <t>Rear Inner Spar</t>
+  </si>
+  <si>
+    <t>4/0:35</t>
+  </si>
+  <si>
+    <t>Rear Mid Spar</t>
+  </si>
+  <si>
+    <t>9/1:12</t>
+  </si>
+  <si>
+    <t>9/1:11</t>
+  </si>
+  <si>
+    <t>Rear Outer Spar</t>
+  </si>
+  <si>
+    <t>5/0:42</t>
+  </si>
+  <si>
+    <t>Outer Trailing Edge</t>
+  </si>
+  <si>
+    <t>4/1:14</t>
+  </si>
+  <si>
+    <t>Mid Trailing Edge</t>
+  </si>
+  <si>
+    <t>4/1:10</t>
+  </si>
+  <si>
+    <t>Inner Trailing Edge</t>
+  </si>
+  <si>
+    <t>4/1:12</t>
+  </si>
+  <si>
+    <t>Version 3</t>
+  </si>
+  <si>
+    <t>Version 4</t>
+  </si>
+  <si>
+    <t>Version 5</t>
+  </si>
+  <si>
+    <t>Version 6</t>
+  </si>
+  <si>
+    <t>Version 7</t>
+  </si>
+  <si>
+    <t>Version 8</t>
+  </si>
+  <si>
+    <t>Version 9</t>
+  </si>
+  <si>
+    <t>Version 10</t>
+  </si>
+  <si>
+    <t>Version 11</t>
+  </si>
+  <si>
+    <t>w/ Supports</t>
+  </si>
+  <si>
+    <t>Rib 1 w/o Support</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,8 +350,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,8 +370,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -259,11 +453,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -277,11 +620,481 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="26">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -300,6 +1113,17 @@
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{B3B5CC73-7FC8-4C2B-9B3D-6062A380FDA6}" name="Object"/>
     <tableColumn id="2" xr3:uid="{F0B453FF-DDA5-4D53-9A49-3E28A67081AF}" name="Mass (g)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{A1788C5E-740A-4939-9C59-B3C2CF35DE48}" name="Table411" displayName="Table411" ref="E5:F16" totalsRowShown="0">
+  <autoFilter ref="E5:F16" xr:uid="{A1788C5E-740A-4939-9C59-B3C2CF35DE48}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{E7BA2C23-EE0D-48D0-8DBA-9ECFCDB718E6}" name="Object"/>
+    <tableColumn id="2" xr3:uid="{1A2C6144-1E51-4613-A2BF-A592EEF1771F}" name="Cost ($)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -350,6 +1174,48 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{027D01CA-8610-4345-8080-A1CD5C2188E3}" name="Table7" displayName="Table7" ref="A6:L50" totalsRowShown="0" tableBorderDxfId="25">
+  <autoFilter ref="A6:L50" xr:uid="{027D01CA-8610-4345-8080-A1CD5C2188E3}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{0AED2B6A-46A5-4321-AB11-649F79F3D0B9}" name="Print Object" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{3CE70BBD-3B54-4598-B1F6-CB070D8BD4D8}" name="Version 1" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{12F2F954-D92F-4BC3-8B81-5DE2BE33B90C}" name="Version 2" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{81265B2F-4ED1-49A7-832D-CB906F620E7A}" name="Version 3" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{A7A4C044-289B-4F8F-84E0-5228383B6262}" name="Version 4" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{AF77F938-E80F-4254-8A92-A150282D163A}" name="Version 5" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{7D88C238-1FCF-4AC4-AB6E-2AD3B983C883}" name="Version 6" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{DE77B850-E7EB-44EA-829F-3DD145A74DD4}" name="Version 7" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{985740BC-A390-4BF7-8000-08B9DBDFCEB4}" name="Version 8" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{71A4CAB9-47C0-4006-B8A4-04E1A745B8CC}" name="Version 9" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{6C19270B-B1CC-4700-89F0-F7E8D4BB3D17}" name="Version 10" dataDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{E10DA2D3-47BA-4415-AE49-7DB45B5282E2}" name="Version 11" dataDxfId="13"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{790ECA6C-716B-4E77-91EF-09BC116714FE}" name="Table712" displayName="Table712" ref="A6:L50" totalsRowShown="0" tableBorderDxfId="12">
+  <autoFilter ref="A6:L50" xr:uid="{790ECA6C-716B-4E77-91EF-09BC116714FE}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{5C343FD2-19BA-4882-9D4C-803A265AF068}" name="Print Object" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{B113C689-3915-448B-9AB7-FC0151F9A312}" name="Version 1" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{413B06FA-3829-4C70-B614-13E35C329D16}" name="Version 2" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{43CA958D-5EF9-48B8-A406-B64E01B693A4}" name="Version 3" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{BCA1E467-9122-46F9-8332-ACCEA16AF55A}" name="Version 4" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{D049DFF9-86DD-4240-AEBD-DCB8F5CCE9A2}" name="Version 5" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{E652D227-CFEE-4367-81A9-AACB3E03E502}" name="Version 6" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{C5E7C2AE-E55C-4C18-9323-040525A11E82}" name="Version 7" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{79D67E5D-86F0-4F2F-A50B-29194A9EC622}" name="Version 8" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{5B1CFDFE-AE78-4816-A647-27012AB14CC7}" name="Version 9" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{B6CE62C4-C85A-4C0E-B699-F97E14FCE708}" name="Version 10" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{9463FB2D-57E2-4FC9-A471-E73221D73079}" name="Version 11" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{31EFEA35-DC94-49DB-8F3C-31FA9FEE7EA0}" name="Table29" displayName="Table29" ref="A5:B16" totalsRowShown="0">
   <autoFilter ref="A5:B16" xr:uid="{31EFEA35-DC94-49DB-8F3C-31FA9FEE7EA0}"/>
   <tableColumns count="2">
@@ -360,23 +1226,12 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{EE2C1C97-219D-47EB-BFF4-6B4D16838243}" name="Table310" displayName="Table310" ref="C5:D16" totalsRowShown="0">
   <autoFilter ref="C5:D16" xr:uid="{EE2C1C97-219D-47EB-BFF4-6B4D16838243}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{32AAEC9E-18AA-4FEB-9D7C-E2B8B5117BA8}" name="Object"/>
     <tableColumn id="2" xr3:uid="{37761C63-3D68-4E12-812C-377D98C8FCAE}" name="Cost ($)"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{A1788C5E-740A-4939-9C59-B3C2CF35DE48}" name="Table411" displayName="Table411" ref="E5:F16" totalsRowShown="0">
-  <autoFilter ref="E5:F16" xr:uid="{A1788C5E-740A-4939-9C59-B3C2CF35DE48}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{E7BA2C23-EE0D-48D0-8DBA-9ECFCDB718E6}" name="Object"/>
-    <tableColumn id="2" xr3:uid="{1A2C6144-1E51-4613-A2BF-A592EEF1771F}" name="Cost ($)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -647,8 +1502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1025,6 +1880,1637 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D8631C1-F72F-4DE1-9623-4C1C6EE3B8CC}">
+  <dimension ref="A2:N50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L50" sqref="A5:L50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" customWidth="1"/>
+    <col min="7" max="10" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+    </row>
+    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" t="s">
+        <v>90</v>
+      </c>
+      <c r="G6" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" t="s">
+        <v>93</v>
+      </c>
+      <c r="J6" t="s">
+        <v>94</v>
+      </c>
+      <c r="K6" t="s">
+        <v>95</v>
+      </c>
+      <c r="L6" t="s">
+        <v>96</v>
+      </c>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="11"/>
+    </row>
+    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="13"/>
+    </row>
+    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="11"/>
+    </row>
+    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="13"/>
+    </row>
+    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="11"/>
+    </row>
+    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="13"/>
+    </row>
+    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="13"/>
+    </row>
+    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="11"/>
+    </row>
+    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="13"/>
+    </row>
+    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="11"/>
+    </row>
+    <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="13"/>
+    </row>
+    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="11"/>
+    </row>
+    <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="13"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="11"/>
+    </row>
+    <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="13"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="11"/>
+    </row>
+    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="13"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A25" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="11"/>
+    </row>
+    <row r="26" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="13"/>
+    </row>
+    <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="11"/>
+    </row>
+    <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="13"/>
+    </row>
+    <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="11"/>
+    </row>
+    <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="13"/>
+    </row>
+    <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="11"/>
+    </row>
+    <row r="32" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="13"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A33" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="11"/>
+    </row>
+    <row r="34" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="13"/>
+    </row>
+    <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="11"/>
+    </row>
+    <row r="36" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="13"/>
+    </row>
+    <row r="37" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="11"/>
+    </row>
+    <row r="38" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="13"/>
+    </row>
+    <row r="39" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="11"/>
+    </row>
+    <row r="40" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="12"/>
+      <c r="K40" s="12"/>
+      <c r="L40" s="13"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A41" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
+      <c r="L41" s="11"/>
+    </row>
+    <row r="42" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="12"/>
+      <c r="K42" s="12"/>
+      <c r="L42" s="13"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A43" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="10"/>
+      <c r="K43" s="10"/>
+      <c r="L43" s="11"/>
+    </row>
+    <row r="44" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="12"/>
+      <c r="J44" s="12"/>
+      <c r="K44" s="12"/>
+      <c r="L44" s="13"/>
+    </row>
+    <row r="45" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="10"/>
+      <c r="K45" s="10"/>
+      <c r="L45" s="11"/>
+    </row>
+    <row r="46" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="12"/>
+      <c r="K46" s="12"/>
+      <c r="L46" s="13"/>
+    </row>
+    <row r="47" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="10"/>
+      <c r="K47" s="10"/>
+      <c r="L47" s="11"/>
+    </row>
+    <row r="48" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="12"/>
+      <c r="J48" s="12"/>
+      <c r="K48" s="12"/>
+      <c r="L48" s="13"/>
+    </row>
+    <row r="49" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="10"/>
+      <c r="K49" s="10"/>
+      <c r="L49" s="11"/>
+    </row>
+    <row r="50" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
+      <c r="J50" s="14"/>
+      <c r="K50" s="14"/>
+      <c r="L50" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A5:L5"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4AA0C21-AB0E-4984-8008-AE93F5440F3E}">
+  <dimension ref="A4:L50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="21"/>
+    </row>
+    <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" t="s">
+        <v>90</v>
+      </c>
+      <c r="G6" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" t="s">
+        <v>93</v>
+      </c>
+      <c r="J6" t="s">
+        <v>94</v>
+      </c>
+      <c r="K6" t="s">
+        <v>95</v>
+      </c>
+      <c r="L6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="15"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="11"/>
+    </row>
+    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="13"/>
+    </row>
+    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="15"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="11"/>
+    </row>
+    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="13"/>
+    </row>
+    <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="15"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="11"/>
+    </row>
+    <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="13"/>
+    </row>
+    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="15"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="13"/>
+    </row>
+    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="15"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="11"/>
+    </row>
+    <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="13"/>
+    </row>
+    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="15"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="11"/>
+    </row>
+    <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="13"/>
+    </row>
+    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="15"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="11"/>
+    </row>
+    <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="10"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="13"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21" s="15"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="11"/>
+    </row>
+    <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="13"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" s="15"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="11"/>
+    </row>
+    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="13"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A25" s="15"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="11"/>
+    </row>
+    <row r="26" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="13"/>
+    </row>
+    <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="15"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="11"/>
+    </row>
+    <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" s="10"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="13"/>
+    </row>
+    <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="15"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="11"/>
+    </row>
+    <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" s="10"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="13"/>
+    </row>
+    <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="15"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="11"/>
+    </row>
+    <row r="32" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" s="10"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="13"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A33" s="15"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="11"/>
+    </row>
+    <row r="34" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="13"/>
+    </row>
+    <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="15"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="11"/>
+    </row>
+    <row r="36" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" s="10"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="13"/>
+    </row>
+    <row r="37" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="15"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="11"/>
+    </row>
+    <row r="38" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B38" s="10"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="13"/>
+    </row>
+    <row r="39" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="15"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="11"/>
+    </row>
+    <row r="40" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" s="10"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="12"/>
+      <c r="K40" s="12"/>
+      <c r="L40" s="13"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A41" s="15"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
+      <c r="L41" s="11"/>
+    </row>
+    <row r="42" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="12"/>
+      <c r="K42" s="12"/>
+      <c r="L42" s="13"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A43" s="15"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="10"/>
+      <c r="K43" s="10"/>
+      <c r="L43" s="11"/>
+    </row>
+    <row r="44" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="12"/>
+      <c r="J44" s="12"/>
+      <c r="K44" s="12"/>
+      <c r="L44" s="13"/>
+    </row>
+    <row r="45" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="15"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="10"/>
+      <c r="K45" s="10"/>
+      <c r="L45" s="11"/>
+    </row>
+    <row r="46" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" s="10"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="12"/>
+      <c r="K46" s="12"/>
+      <c r="L46" s="13"/>
+    </row>
+    <row r="47" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="15"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="10"/>
+      <c r="K47" s="10"/>
+      <c r="L47" s="11"/>
+    </row>
+    <row r="48" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" s="10"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="12"/>
+      <c r="J48" s="12"/>
+      <c r="K48" s="12"/>
+      <c r="L48" s="13"/>
+    </row>
+    <row r="49" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="15"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="10"/>
+      <c r="K49" s="10"/>
+      <c r="L49" s="11"/>
+    </row>
+    <row r="50" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B50" s="10"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
+      <c r="J50" s="14"/>
+      <c r="K50" s="14"/>
+      <c r="L50" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A5:L5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3C7A39F-1EB6-427B-9329-0D14A0290A39}">
   <dimension ref="A1:F16"/>
   <sheetViews>

</xml_diff>